<commit_message>
Update Solution.xlsx. Add a fact.
</commit_message>
<xml_diff>
--- a/Solution.xlsx
+++ b/Solution.xlsx
@@ -74,8 +74,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Numerujemy wszystkie wierzchołki.
-Iterujemy od najmniejszego wierzchołka do największego.
-Szukamy wszystkich ścieżek od wierzchołka na którym jesteśmy do wierzchołka o liczbie największej. 
+Iterujemy od wierzchołka o numerze najmniejszym do wierzchołka o numerze największym.
+Szukamy wszystkich ścieżek od numeru wierzchołka dla którego obliczamy sumę ścieżek w danej iteracji do wierzchołka o numerze największym poprzez wykorzystanie algorytmu Deep First Search. 
 </t>
         </r>
       </text>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t xml:space="preserve">Fakty</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t xml:space="preserve">Algorytmy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testowanie</t>
   </si>
   <si>
     <t xml:space="preserve">Ilość wierzchołków</t>
@@ -106,7 +109,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">A</t>
+      <t xml:space="preserve">V</t>
     </r>
     <r>
       <rPr>
@@ -116,7 +119,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">n </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -154,12 +157,40 @@
     <t xml:space="preserve">Brutalny</t>
   </si>
   <si>
+    <t xml:space="preserve">Czasowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pamięciowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poprawnościowe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maksymalnie 3 krawędzie na wierzchołek</t>
   </si>
   <si>
+    <t xml:space="preserve">cProfile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory-profiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unittest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Początkowy stan jest kopiowany czterokrotnie i scalany przez dwa dodane wierzchołki, których krawędzie mają taką samą, określoną wartość</t>
   </si>
   <si>
+    <t xml:space="preserve">Pozwala na kalibrację profilowania, przez co ograniczany jest wpływ profilowania na wyniki czasu wykonywania.
+Przedstawia wpływ czasowy poszczególnych funkcji na działanie programu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Przedstawia wpływ pamięciowy poszczególnych funkcji na działanie programu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testy jednostkowe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Symetria względem poziomu</t>
   </si>
   <si>
@@ -169,7 +200,7 @@
     <t xml:space="preserve">Wierzchołki dodawane mają zawsze 3 krawędzie</t>
   </si>
   <si>
-    <t xml:space="preserve">Wierzchołki liściasto-scalające mają zawsze 2 krawędzie</t>
+    <t xml:space="preserve">Wierzchołki scalające, należące do poprzedniego grafu mają zawsze 2 krawędzie</t>
   </si>
   <si>
     <t xml:space="preserve">Przeszukiwanie</t>
@@ -178,12 +209,12 @@
     <t xml:space="preserve">DFS</t>
   </si>
   <si>
-    <t xml:space="preserve">Zaznaczanie przebytego wierzchołka?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pre-order</t>
   </si>
   <si>
+    <t xml:space="preserve">Po obliczeniu sumy ścieżek w grafie i potem dodaniu wierzchołka do tego grafu, suma ścieżek dla tego wierzchołka będzie równa sumie ścieżek dla sąsiadującego wierzchołka plus ilość wierzchołków pomnożona przez koszt krawędzi dodanej do grafu.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Numerowanie</t>
   </si>
   <si>
@@ -197,10 +228,20 @@
   </si>
   <si>
     <t xml:space="preserve">Graf jako lista zbiorów. Poszczególne zbiory reprezentują wierzchołki. W zbiorach znajdują się numery wierzchołków, z którymi dany wierzchołek jest połączony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilość krawędzi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E = V-1</t>
   </si>
   <si>
     <t xml:space="preserve">Alternatywa:
 Specjalne klasy o nazwie Vertex oraz Edge. W liście trzymane są Vertex. Edge posiada 2 Vertex oraz wartość.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rozwiązanie właściwe: 
+Graf jako lista wierzchołków. Indeks wierzchołka zgadza się z numerem wierzchołka. Każdy wierzchołek posiada listę krawędzi. Krawędź jest reprezentowana jako krotka której pierwszym elementem jest wierzchołek będący drugim końcem krawędzi, a drugim elementem jest wartość tej krawędzi.</t>
   </si>
 </sst>
 </file>
@@ -247,7 +288,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,7 +298,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFED1C24"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFF04E4D"/>
       </patternFill>
     </fill>
     <fill>
@@ -268,8 +309,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5565AF"/>
-        <bgColor rgb="FF3366FF"/>
+        <fgColor rgb="FF0066B3"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
@@ -284,8 +325,14 @@
         <bgColor rgb="FFCC99FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF04E4D"/>
+        <bgColor rgb="FFED1C24"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -307,13 +354,6 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -373,19 +413,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,7 +462,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0066B3"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -445,8 +485,8 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF5565AF"/>
+      <rgbColor rgb="FFF04E4D"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFBD7CB5"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF62A73B"/>
@@ -466,17 +506,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,192 +534,300 @@
       <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="H2" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8"/>
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
+      <c r="J3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="D4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="J4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="8"/>
+      <c r="A9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9"/>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="0" t="s">
-        <v>15</v>
-      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="D11" s="10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="9"/>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="D14" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="D15" s="10" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="D16" s="10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="D17" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="A20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="D23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="26">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:F1"/>
+    <mergeCell ref="J1:L1"/>
     <mergeCell ref="D2:F3"/>
     <mergeCell ref="A3:B4"/>
     <mergeCell ref="D4:F7"/>
+    <mergeCell ref="J4:J18"/>
+    <mergeCell ref="K4:K10"/>
+    <mergeCell ref="L4:L5"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="A9:B11"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A12:B19"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D14:F14"/>
@@ -686,6 +836,7 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F22"/>
     <mergeCell ref="D23:F27"/>
+    <mergeCell ref="D28:F36"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>